<commit_message>
new fields at UsuarioAWS.CSV and .XLSX and new file that have policy sample
</commit_message>
<xml_diff>
--- a/iam/UsuariosAWS.xlsx
+++ b/iam/UsuariosAWS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Documents\Pessoal\The Cloud Bootcamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Documents\Pessoal\The Cloud Bootcamp\tcb-aws-mod2-challenge\iam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC75AAEC-4357-4C13-B303-0F0EEAA15264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0182647F-4EBA-4F72-8838-F2BC2A544F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC25B4AE-5C94-48A9-ACA7-C318FE476ADA}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="100">
   <si>
     <t>Geraldo Benedito Rocha</t>
   </si>
@@ -245,18 +245,9 @@
     <t>0ZGnJiwX9l</t>
   </si>
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Senha</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
     <t>geraldobeneditorocha@jsagromecanica.com.br</t>
   </si>
   <si>
@@ -330,6 +321,33 @@
   </si>
   <si>
     <t>alexandrecauaaugustogomes@comdados.com</t>
+  </si>
+  <si>
+    <t>Policy</t>
+  </si>
+  <si>
+    <t>CloudAdmins</t>
+  </si>
+  <si>
+    <t>CloudDBAs</t>
+  </si>
+  <si>
+    <t>CloudReadOnly</t>
+  </si>
+  <si>
+    <t>EnforceMFAPolicy</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -403,27 +421,31 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_1" connectionId="2" xr16:uid="{1D5D1703-523D-405B-BD7E-260B4D150732}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="5" unboundColumnsRight="1">
-    <queryTableFields count="4">
+  <queryTableRefresh nextId="7" unboundColumnsRight="3">
+    <queryTableFields count="6">
       <queryTableField id="1" name="Column1.nome" tableColumnId="1"/>
       <queryTableField id="2" name="Column1.email" tableColumnId="2"/>
       <queryTableField id="3" name="Column1.senha" tableColumnId="3"/>
       <queryTableField id="4" dataBound="0" tableColumnId="4"/>
+      <queryTableField id="5" dataBound="0" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98D5E5FB-2196-4BC1-A898-5C250AE6C223}" name="pessoas__2" displayName="pessoas__2" ref="A1:D31" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D31" xr:uid="{98D5E5FB-2196-4BC1-A898-5C250AE6C223}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7832B7DA-F16F-46E1-AFD7-F7285429BA8E}" uniqueName="1" name="Nome" queryTableFieldId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98D5E5FB-2196-4BC1-A898-5C250AE6C223}" name="pessoas__2" displayName="pessoas__2" ref="A1:F31" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F31" xr:uid="{98D5E5FB-2196-4BC1-A898-5C250AE6C223}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7832B7DA-F16F-46E1-AFD7-F7285429BA8E}" uniqueName="1" name="Name" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{FC4135DA-9932-4A4F-B295-3ECBE7AD8855}" uniqueName="2" name="Email" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{26C516AE-DD35-4A90-8B84-B32AE1DEB56D}" uniqueName="3" name="Senha" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{D145E87B-CAEF-4439-87BA-6F96C12ECF0A}" uniqueName="4" name="Usuario" queryTableFieldId="4" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{26C516AE-DD35-4A90-8B84-B32AE1DEB56D}" uniqueName="3" name="Password" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{D145E87B-CAEF-4439-87BA-6F96C12ECF0A}" uniqueName="4" name="User" queryTableFieldId="4" dataDxfId="0">
       <calculatedColumnFormula>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" xr3:uid="{AF4AF636-793F-4677-B254-11A635F747AE}" uniqueName="5" name="Group" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{ECC80D07-D55E-432A-A2E2-A370C2F2D85E}" uniqueName="6" name="Policy" queryTableFieldId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82DA80D-CD32-487E-9212-AD7C49D50DA2}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,28 +760,36 @@
     <col min="2" max="2" width="78.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -768,8 +798,14 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>geraldobeneditorocha</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -783,8 +819,14 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>ssuelieloarezende</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -798,13 +840,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>rraimundofabiotomasnovaes</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -813,13 +861,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>daianedanielaallananunes88</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -828,8 +882,14 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>sophiafranciscadepaula</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -843,13 +903,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>iisismanuelamalubarros</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -858,13 +924,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>mateusjoaquimsergiocarvalho</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -873,13 +945,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>adrianaelaineramos</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -888,13 +966,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>tiagomanoelpereira</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -903,13 +987,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>antonellalopes</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -918,13 +1008,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>sarezende</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -933,13 +1029,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>nelsonjorgedepaula96</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -948,13 +1050,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>andersoncaualopes</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -963,13 +1071,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>gabrielavitoriarosangelacortereal</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -978,13 +1092,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>alexandrecauaaugustogomes</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
@@ -993,8 +1113,14 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>otavioiagobarros</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1008,13 +1134,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>eelzarafaelagalvao</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -1023,13 +1155,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>amandaagathagiovannaalmada85</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
@@ -1038,13 +1176,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>auroragiovanasarahdacosta</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -1053,13 +1197,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>beatrizmarianealmada80</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
         <v>45</v>
@@ -1068,13 +1218,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>vitoriajoanacaldeira</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
@@ -1083,8 +1239,14 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>isabellyyasmindrumond</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1098,13 +1260,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>ttiagoyurimoreira</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
@@ -1113,13 +1281,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>julialarissanogueira</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
         <v>54</v>
@@ -1128,13 +1302,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>nairsophieemilyalves</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
@@ -1143,13 +1323,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>marinaalicehelenadaluz</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
         <v>58</v>
@@ -1158,13 +1344,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>valentinasophiabernardes</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
@@ -1173,13 +1365,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>renatofilipedamata</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
         <v>62</v>
@@ -1188,13 +1386,19 @@
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>juansamuelsebastiaodossantos</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
         <v>64</v>
@@ -1202,6 +1406,12 @@
       <c r="D31" t="str">
         <f>LEFT(pessoas__2[[#This Row],[Email]],SEARCH("@",pessoas__2[[#This Row],[Email]])-1)</f>
         <v>anaceciliadamota</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>